<commit_message>
Initial working category axis.
</commit_message>
<xml_diff>
--- a/test/functional/xlsx_files/chart_bar01.xlsx
+++ b/test/functional/xlsx_files/chart_bar01.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -67,7 +67,7 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
-          <c:val>
+          <c:cat>
             <c:numRef>
               <c:f>Sheet1!$A$1:$A$5</c:f>
               <c:numCache>
@@ -90,11 +90,7 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>Sheet1!$B$1:$B$5</c:f>
@@ -120,24 +116,77 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="50010001"/>
-        <c:axId val="50010002"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$1:$A$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$1:$C$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>15</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:axId val="64052224"/>
+        <c:axId val="64055552"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="50010001"/>
+        <c:axId val="64052224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="50010002"/>
+        <c:crossAx val="64055552"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="50010002"/>
+        <c:axId val="64055552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -145,7 +194,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="50010001"/>
+        <c:crossAx val="64052224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>

</xml_diff>